<commit_message>
adding a function to compare h to optimum
</commit_message>
<xml_diff>
--- a/runningArea/30Missions.xlsx
+++ b/runningArea/30Missions.xlsx
@@ -5595,7 +5595,7 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="B23">
         <v>7</v>
@@ -5612,7 +5612,7 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="B24">
         <v>0</v>
@@ -5629,7 +5629,7 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="B25">
         <v>13</v>
@@ -5646,7 +5646,7 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="B26">
         <v>0</v>
@@ -5663,7 +5663,7 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="B27">
         <v>26</v>
@@ -5680,7 +5680,7 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="B28">
         <v>0</v>
@@ -5697,7 +5697,7 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="B29">
         <v>12</v>
@@ -5714,7 +5714,7 @@
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="B30">
         <v>0</v>
@@ -5731,7 +5731,7 @@
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="B31">
         <v>29</v>
@@ -5748,7 +5748,7 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="B32">
         <v>0</v>
@@ -5765,7 +5765,7 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="B33">
         <v>17</v>
@@ -5782,7 +5782,7 @@
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="B34">
         <v>8</v>
@@ -5799,7 +5799,7 @@
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="B35">
         <v>0</v>
@@ -5816,7 +5816,7 @@
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="B36">
         <v>30</v>
@@ -5833,7 +5833,7 @@
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="B37">
         <v>0</v>
@@ -5850,7 +5850,7 @@
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="B38">
         <v>32</v>
@@ -5867,7 +5867,7 @@
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="B39">
         <v>0</v>
@@ -5884,7 +5884,7 @@
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="B40">
         <v>19</v>
@@ -5901,7 +5901,7 @@
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="B41">
         <v>20</v>
@@ -5918,7 +5918,7 @@
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="B42">
         <v>0</v>
@@ -5935,7 +5935,7 @@
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="B43">
         <v>21</v>
@@ -5952,7 +5952,7 @@
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B44">
         <v>34</v>
@@ -5969,7 +5969,7 @@
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B45">
         <v>0</v>
@@ -5986,7 +5986,7 @@
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B46">
         <v>16</v>
@@ -6003,7 +6003,7 @@
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B47">
         <v>0</v>
@@ -6020,7 +6020,7 @@
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B48">
         <v>22</v>
@@ -6037,7 +6037,7 @@
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B49">
         <v>0</v>
@@ -6054,7 +6054,7 @@
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B50">
         <v>24</v>
@@ -6071,7 +6071,7 @@
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B51">
         <v>0</v>
@@ -6088,7 +6088,7 @@
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B52">
         <v>6</v>
@@ -6105,7 +6105,7 @@
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B53">
         <v>36</v>
@@ -6122,7 +6122,7 @@
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B54">
         <v>0</v>
@@ -6139,7 +6139,7 @@
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B55">
         <v>23</v>
@@ -6156,7 +6156,7 @@
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B56">
         <v>0</v>
@@ -6173,7 +6173,7 @@
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B57">
         <v>5</v>
@@ -6190,7 +6190,7 @@
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B58">
         <v>38</v>
@@ -6207,7 +6207,7 @@
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B59">
         <v>35</v>
@@ -6224,7 +6224,7 @@
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B60">
         <v>18</v>
@@ -6241,7 +6241,7 @@
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B61">
         <v>0</v>
@@ -6258,7 +6258,7 @@
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B62">
         <v>37</v>
@@ -6275,7 +6275,7 @@
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B63">
         <v>0</v>
@@ -6292,7 +6292,7 @@
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B64">
         <v>31</v>

</xml_diff>